<commit_message>
Updated aiphoria_scenario_file_template.xlsx to include fill_method and simple first-order decay function.
</commit_message>
<xml_diff>
--- a/template/aiphoria_scenario_file_template.xlsx
+++ b/template/aiphoria_scenario_file_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\ForestPaths_ODYM\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D92FC66-F68D-4CF6-857D-7E973C7DB973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED760FD-A258-466E-BE37-168B9A20C632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="10" r:id="rId1"/>
@@ -47,24 +47,6 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={E0420DE5-0C68-4247-A968-F7ADA1450266}</author>
-  </authors>
-  <commentList>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{E0420DE5-0C68-4247-A968-F7ADA1450266}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Sankey diagram process positioning</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
     <author>tc={00ACE76D-287A-45EC-B71C-BD8339701482}</author>
   </authors>
   <commentList>
@@ -81,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="157">
   <si>
     <t>Years</t>
   </si>
@@ -173,9 +155,15 @@
     <t xml:space="preserve">float </t>
   </si>
   <si>
+    <t xml:space="preserve">Scenarios </t>
+  </si>
+  <si>
     <t>Please note</t>
   </si>
   <si>
+    <t>Dynamic case (multiple years with different scenarios)</t>
+  </si>
+  <si>
     <t>Process IDs</t>
   </si>
   <si>
@@ -204,6 +192,18 @@
   </si>
   <si>
     <t>Make sure that no whitespaces exist on the process IDs (at the end or beginning)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the system is not balanced (Inputs not equal to outputs) then aiphoria creates virtual flows to show the imbalances. Virtual flows can toggled off from the notebook. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must filled in cells </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cells to fill for running aiphoria </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please check the starred (*) cells on the processes and flows sheets. </t>
   </si>
   <si>
     <t>General information</t>
@@ -381,6 +381,9 @@
     <t>c</t>
   </si>
   <si>
+    <t xml:space="preserve">https://excalidraw.com/#json=acMq06Ek074LvgJQcBgt-,_z-k-OWtxYKdxCtl_tJVQg </t>
+  </si>
+  <si>
     <t xml:space="preserve">tuple </t>
   </si>
   <si>
@@ -481,6 +484,32 @@
     <t xml:space="preserve">This is the input file of aiphoria where the user defines the processes/nodes and flows/arrows/edges within the preferred system. aiphoria supports both static and dynamic assessments (e.g from 2021 to 2050). If can be used to assess any system and both product or process based MFAs. </t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">If the user wants to run different scenarios using relative value (shares) for the same process, they should add multiple flows (rows) on the flow sheet indicating the change in the value cell (e.g P3:EU -&gt; P5:EU and  value: 100% in 2021 and  P3:EU -&gt; P5:EU and value 50% in 2022). If the scenarios when using relative value (shares) remain the same throughtout the timeline indicated by the user; then aiphoria is </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>repeating the value given for the last year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. P3:EU -&gt; P5:EU with value: 50%)  </t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">The carbon fraction sheet is only temprorary here and it is being used by thee Flows sheet. In the next version of aiphoria this will be moved. </t>
   </si>
   <si>
@@ -580,31 +609,43 @@
     <t>Distribution type</t>
   </si>
   <si>
+    <t>fill_missing_absolute_flows</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Fill in missing timestep with the last timestep provided by the user. Default value is True</t>
+  </si>
+  <si>
+    <t>fill_missing_relative_flows</t>
+  </si>
+  <si>
+    <t>fill_method</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
     <t xml:space="preserve">String </t>
   </si>
   <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>Float</t>
-  </si>
-  <si>
-    <t>fill_missing_absolute_flows</t>
-  </si>
-  <si>
-    <t>fill_missing_relative_flows</t>
-  </si>
-  <si>
-    <t>Fill in missing timestep with the last timestep provided by the user. Default value is True</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the system is not balanced (Inputs not equal to outputs) then aiphoria creates virtual flows to show the imbalances. Virtual flows can toggled off from Settings. </t>
+    <t>Interpolate</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeros </t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Type of fill method</t>
   </si>
 </sst>
 </file>
@@ -614,7 +655,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,6 +701,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -832,13 +881,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -859,22 +908,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -916,6 +950,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>779319</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>64064</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>314785</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>16634</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Graphic 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{060A53AB-2C39-4786-AA4D-FFB36F5549BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5004955" y="4618746"/>
+          <a:ext cx="9594155" cy="2723479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1221,14 +1310,6 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="P3" dT="2024-07-11T08:34:08.99" personId="{10F4E90A-0171-4D8D-A06D-5391EEA853D3}" id="{E0420DE5-0C68-4247-A968-F7ADA1450266}">
-    <text>Sankey diagram process positioning</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="P3" dT="2024-07-05T06:41:30.02" personId="{10F4E90A-0171-4D8D-A06D-5391EEA853D3}" id="{00ACE76D-287A-45EC-B71C-BD8339701482}">
     <text>Conversion to ODMT not carbon!</text>
   </threadedComment>
@@ -1237,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8D2205-82D8-4539-BF3B-F097E196F1D1}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1252,7 +1333,7 @@
     <col min="5" max="16384" width="9.1796875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -1264,7 +1345,7 @@
       </c>
       <c r="D1" s="39"/>
     </row>
-    <row r="2" spans="1:4" ht="156" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="156" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -1272,11 +1353,12 @@
         <v>6</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D2" s="40"/>
-    </row>
-    <row r="3" spans="1:4" ht="203.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="203.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
@@ -1284,115 +1366,139 @@
         <v>7</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D3" s="40"/>
     </row>
-    <row r="4" spans="1:4" s="17" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="17" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" s="41"/>
     </row>
-    <row r="5" spans="1:4" s="17" customFormat="1" ht="96.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="17" customFormat="1" ht="96.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D5" s="41"/>
     </row>
-    <row r="6" spans="1:4" ht="145" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="145" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="38"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="42"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="D7" s="38"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="42"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="38"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="42"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+      <c r="B9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="42"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="38"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="38"/>
-    </row>
-    <row r="11" spans="1:4" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
-        <v>69</v>
+      <c r="D10" s="42"/>
+    </row>
+    <row r="11" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="D11" s="38"/>
     </row>
-    <row r="12" spans="1:4" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:4" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="38"/>
+    </row>
+    <row r="13" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="38"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
@@ -1407,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B48F50B1-BB9C-4949-B068-97B97AFD08C4}">
-  <dimension ref="B2:E20"/>
+  <dimension ref="B2:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1422,17 +1528,17 @@
   <sheetData>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.5">
       <c r="B2" s="37" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="36" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
@@ -1440,13 +1546,13 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="35" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>4</v>
@@ -1454,198 +1560,187 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C7" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="34" t="s">
-        <v>136</v>
-      </c>
+      <c r="D7" s="34"/>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>136</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D8" s="34"/>
       <c r="E8" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C9" s="32">
         <v>2</v>
       </c>
-      <c r="D9" s="32" t="s">
-        <v>137</v>
-      </c>
+      <c r="D9" s="32"/>
       <c r="E9" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="34" t="s">
-        <v>138</v>
-      </c>
+      <c r="D10" s="34"/>
       <c r="E10" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>138</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D11" s="34"/>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C12" s="32">
         <v>2</v>
       </c>
-      <c r="D12" s="32" t="s">
-        <v>137</v>
-      </c>
+      <c r="D12" s="32"/>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C13" s="32">
         <v>2021</v>
       </c>
-      <c r="D13" s="32" t="s">
-        <v>137</v>
-      </c>
+      <c r="D13" s="32"/>
       <c r="E13" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C14" s="32">
         <v>2030</v>
       </c>
-      <c r="D14" s="32" t="s">
-        <v>137</v>
-      </c>
+      <c r="D14" s="32"/>
       <c r="E14" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C15" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="D15" t="s">
-        <v>139</v>
-      </c>
+      <c r="D15" s="32"/>
       <c r="E15" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C16" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="D16" t="s">
-        <v>139</v>
-      </c>
+      <c r="D16" s="32"/>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C17" s="31">
         <v>0.1</v>
       </c>
-      <c r="D17" s="32" t="s">
-        <v>140</v>
-      </c>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C18" s="30">
         <v>3.67</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>140</v>
-      </c>
+      <c r="D18" s="30"/>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C19" s="33" t="b">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E19" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C20" s="33" t="b">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E20" t="s">
-        <v>143</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1666,20 +1761,32 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C19:C20" xr:uid="{0304884E-2763-4109-832F-B724E299E82B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C19:C20" xr:uid="{5D3B6C52-629A-48C0-B345-97745DEAC80B}">
       <formula1>Boolean</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{624030A8-D670-4ECF-A910-6FB291FB46D7}">
+          <x14:formula1>
+            <xm:f>Sheet1!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1723,7 +1830,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>11</v>
@@ -1782,28 +1889,28 @@
     <row r="3" spans="1:18" s="27" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="25"/>
       <c r="B3" s="26" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="J3" s="26" t="s">
         <v>16</v>
@@ -1830,7 +1937,7 @@
         <v>27</v>
       </c>
       <c r="R3" s="26" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.4">
@@ -1838,10 +1945,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT(B4,":",C4)</f>
@@ -1854,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1867,7 +1974,7 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="R4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.4">
@@ -1875,10 +1982,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5:D6" si="0">_xlfn.CONCAT(B5,":",C5)</f>
@@ -1891,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1904,7 +2011,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="R5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -1912,23 +2019,23 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>Residues:FI</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1940,7 +2047,7 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="R6" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -1948,10 +2055,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ref="D7" si="1">_xlfn.CONCAT(B7,":",C7)</f>
@@ -1964,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -1976,25 +2083,25 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="R7" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution parameters" prompt="tuple = number or list of parameters separated by comma. Example: for stddev only number! e.g., 1. For shape and scale list separated by comma e.g., shape=1, scale=1.5" sqref="I4" xr:uid="{D124036C-F0AC-436A-866C-354CA25FBBC5}"/>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution parameters" prompt="tuple = number or list of parameters separated by comma. Example: stddev=1. For shape and scale list separated by comma e.g., shape=1, scale=1.5" sqref="I4:I1048576" xr:uid="{93136A82-DC6C-4705-B31C-84E2F453E4FD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Process positioning for the Sankey diagram. Once Sankey has been launched, information can be collected. " sqref="P1:P1048576 Q1:Q1048576" xr:uid="{E664A26A-3D1C-44AC-9797-E891A0E00233}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution type" prompt="Distribution type for stock outflows (=decay). _x000a_-Fixed only uses lifetimes so no parameter is used._x000a_-Normal, LogNormal, FoldedNormal use standard deviation. _x000a_-Weibull uses shape and scale. " xr:uid="{1B854FDE-0BAE-42E5-8C60-482CEE80872A}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution type" prompt="Distribution type for stock outflows (=decay). _x000a_-Fixed only uses lifetimes so no parameter is used._x000a_-Simple only uses lifetimes so no parameter is used._x000a_-Normal, LogNormal, FoldedNormal use standard deviation. _x000a_-Weibull uses shape and scale. " xr:uid="{1B854FDE-0BAE-42E5-8C60-482CEE80872A}">
           <x14:formula1>
-            <xm:f>Sheet1!$C$2:$C$6</xm:f>
+            <xm:f>Sheet1!$C$2:$C$7</xm:f>
           </x14:formula1>
           <xm:sqref>H4:H1048576</xm:sqref>
         </x14:dataValidation>
@@ -2009,7 +2116,7 @@
   <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2112,7 +2219,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -2121,7 +2228,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
@@ -2130,61 +2237,61 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="20" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="M3" s="20" t="s">
         <v>25</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="R3" s="22" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="S3" s="23" t="s">
         <v>21</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="U3" s="23" t="s">
         <v>21</v>
@@ -2192,27 +2299,27 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C4" t="str">
         <f>+_xlfn.XLOOKUP(H4,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Source</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F4" t="str">
         <f>+_xlfn.XLOOKUP(I4,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H4" s="4" t="str">
         <f t="shared" ref="H4:H6" si="0">_xlfn.CONCAT(B4,":",D4)</f>
@@ -2226,45 +2333,45 @@
         <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="L4">
         <v>2021</v>
       </c>
       <c r="N4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="P4">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C5" t="str">
         <f>+_xlfn.XLOOKUP(H5,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F5" t="str">
         <f>+_xlfn.XLOOKUP(I5,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2275,48 +2382,48 @@
         <v>Sawnwood:FI</v>
       </c>
       <c r="J5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="L5">
         <v>2021</v>
       </c>
       <c r="N5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="P5">
         <f>0.4238*'Carbon fraction (will be moved)'!C2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C6" t="str">
         <f>+_xlfn.XLOOKUP(H6,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F6" t="str">
         <f>+_xlfn.XLOOKUP(I6,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>by_prod</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2327,23 +2434,23 @@
         <v>Residues:FI</v>
       </c>
       <c r="J6">
-        <v>10</v>
+        <v>19.5</v>
       </c>
       <c r="K6" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="L6">
         <v>2021</v>
       </c>
       <c r="N6" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="P6">
         <f>0.395*'Carbon fraction (will be moved)'!C2</f>
         <v>0.18959999999999999</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -2544,7 +2651,9 @@
       <c r="O44"/>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C45" s="9"/>
+      <c r="C45" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="N45"/>
@@ -2833,10 +2942,12 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1" xr:uid="{44BDC3E8-14C2-47A6-9A94-576E28D9D557}"/>
+    <hyperlink ref="C45" r:id="rId2" location="json=acMq06Ek074LvgJQcBgt-,_z-k-OWtxYKdxCtl_tJVQg " xr:uid="{96378F21-3514-4467-8F52-95C692A9B7F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2862,13 +2973,13 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>0.48</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2878,10 +2989,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1385D0A5-68C9-46A8-897F-5695B3E81330}">
-  <dimension ref="C1:D6"/>
+  <dimension ref="C1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2891,43 +3002,63 @@
     <col min="11" max="11" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C1" s="35" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="E4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>99</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated aiphoria_scenario_file_template.xlsx and removed existing SVGs to respect updated .gitignore
</commit_message>
<xml_diff>
--- a/template/aiphoria_scenario_file_template.xlsx
+++ b/template/aiphoria_scenario_file_template.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClOrfani\PycharmProjects\ForestPaths_ODYM\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\PythonProjects\aiphoria\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED760FD-A258-466E-BE37-168B9A20C632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89519A9D-55F5-4651-8CF4-D742CC2C8574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1000A452-A98F-45C1-B843-91F7F67E097C}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="10" r:id="rId1"/>
     <sheet name="Settings" sheetId="11" r:id="rId2"/>
     <sheet name="Processes" sheetId="6" r:id="rId3"/>
     <sheet name="Flows" sheetId="1" r:id="rId4"/>
-    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId6"/>
+    <sheet name="Scenarios" sheetId="13" r:id="rId5"/>
+    <sheet name="Carbon fraction (will be moved)" sheetId="7" r:id="rId6"/>
+    <sheet name="Data validation parameters" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flows!$B$3:$M$89</definedName>
-    <definedName name="Boolean">Sheet1!$D$2:$D$3</definedName>
+    <definedName name="Boolean">'Data validation parameters'!$D$2:$D$3</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,10 +48,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={00ACE76D-287A-45EC-B71C-BD8339701482}</author>
+    <author>tc={2190F4CE-A9C1-4BF1-8057-C68B26705A49}</author>
   </authors>
   <commentList>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{00ACE76D-287A-45EC-B71C-BD8339701482}">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{2190F4CE-A9C1-4BF1-8057-C68B26705A49}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="173">
   <si>
     <t>Years</t>
   </si>
@@ -155,15 +156,9 @@
     <t xml:space="preserve">float </t>
   </si>
   <si>
-    <t xml:space="preserve">Scenarios </t>
-  </si>
-  <si>
     <t>Please note</t>
   </si>
   <si>
-    <t>Dynamic case (multiple years with different scenarios)</t>
-  </si>
-  <si>
     <t>Process IDs</t>
   </si>
   <si>
@@ -192,18 +187,6 @@
   </si>
   <si>
     <t>Make sure that no whitespaces exist on the process IDs (at the end or beginning)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the system is not balanced (Inputs not equal to outputs) then aiphoria creates virtual flows to show the imbalances. Virtual flows can toggled off from the notebook. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must filled in cells </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cells to fill for running aiphoria </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please check the starred (*) cells on the processes and flows sheets. </t>
   </si>
   <si>
     <t>General information</t>
@@ -381,9 +364,6 @@
     <t>c</t>
   </si>
   <si>
-    <t xml:space="preserve">https://excalidraw.com/#json=acMq06Ek074LvgJQcBgt-,_z-k-OWtxYKdxCtl_tJVQg </t>
-  </si>
-  <si>
     <t xml:space="preserve">tuple </t>
   </si>
   <si>
@@ -484,19 +464,166 @@
     <t xml:space="preserve">This is the input file of aiphoria where the user defines the processes/nodes and flows/arrows/edges within the preferred system. aiphoria supports both static and dynamic assessments (e.g from 2021 to 2050). If can be used to assess any system and both product or process based MFAs. </t>
   </si>
   <si>
+    <t xml:space="preserve">The carbon fraction sheet is only temprorary here and it is being used by thee Flows sheet. In the next version of aiphoria this will be moved. </t>
+  </si>
+  <si>
+    <t>Conversion factor from C to CO2</t>
+  </si>
+  <si>
+    <t>conversion_factor_c_to_co2</t>
+  </si>
+  <si>
+    <t>If using virtual flows, create virtual flow to process if process total inputs and outputs difference is greater than this value</t>
+  </si>
+  <si>
+    <t>virtual_flows_epsilon</t>
+  </si>
+  <si>
+    <t>Use virtual flows. If enabled, creates missing flows for Processes that have imbalance of input and output flows i.e. unreported flows</t>
+  </si>
+  <si>
+    <t>use_virtual_flows</t>
+  </si>
+  <si>
+    <t>Detect the year range automatically from file</t>
+  </si>
+  <si>
+    <t>detect_year_range</t>
+  </si>
+  <si>
+    <t>Ending year of the model, included in in time range</t>
+  </si>
+  <si>
+    <t>end_year</t>
+  </si>
+  <si>
+    <t>Starting year of the model</t>
+  </si>
+  <si>
+    <t>start_year</t>
+  </si>
+  <si>
+    <t>Number of rows to skip when reading data for Processes (e.g. 2). NOTE: Header row must be the first row to read!</t>
+  </si>
+  <si>
+    <t>skip_num_rows_flows</t>
+  </si>
+  <si>
+    <t>Start column name and end column name separated by colon (e.g. B:R) that contain data for Flows</t>
+  </si>
+  <si>
+    <t>B:U</t>
+  </si>
+  <si>
+    <t>column_range_flows</t>
+  </si>
+  <si>
+    <t>Sheet name that contains data for Flows, (e.g. Flows)</t>
+  </si>
+  <si>
+    <t>sheet_name_flows</t>
+  </si>
+  <si>
+    <t>skip_num_rows_processes</t>
+  </si>
+  <si>
+    <t>Start column name and end column name separated by colon (e.g. B:R) that contain data for Processes</t>
+  </si>
+  <si>
+    <t>B:R</t>
+  </si>
+  <si>
+    <t>column_range_processes</t>
+  </si>
+  <si>
+    <t>Sheet name that contains data for Processes, e.g. (Processes)</t>
+  </si>
+  <si>
+    <t>sheet_name_processes</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Parameter name</t>
+  </si>
+  <si>
+    <t>Example: first parameter sheet_name_processes goes to cell B6 and value Processes goes to cell C6.</t>
+  </si>
+  <si>
+    <t>NOTE: The parameters are read columns B and C and from row 7 downward, including that row.</t>
+  </si>
+  <si>
+    <t>These are the settings for the scenario file</t>
+  </si>
+  <si>
+    <t>Boolean values</t>
+  </si>
+  <si>
+    <t>Distribution type</t>
+  </si>
+  <si>
+    <t>fill_missing_absolute_flows</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Fill in missing timestep with the last timestep provided by the user. Default value is True</t>
+  </si>
+  <si>
+    <t>fill_missing_relative_flows</t>
+  </si>
+  <si>
+    <t>fill_method</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String </t>
+  </si>
+  <si>
+    <t>Interpolate</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeros </t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the system is not balanced (Inputs not equal to outputs) then aiphoria creates virtual flows to show the imbalances. Virtual flows can toggled off from Settings. </t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">If the user wants to run different scenarios using relative value (shares) for the same process, they should add multiple flows (rows) on the flow sheet indicating the change in the value cell (e.g P3:EU -&gt; P5:EU and  value: 100% in 2021 and  P3:EU -&gt; P5:EU and value 50% in 2022). If the scenarios when using relative value (shares) remain the same throughtout the timeline indicated by the user; then aiphoria is </t>
+      <t xml:space="preserve">Fill method if either </t>
     </r>
     <r>
       <rPr>
-        <u/>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>repeating the value given for the last year</t>
+      <t>fill_missing_absolute_flows</t>
     </r>
     <r>
       <rPr>
@@ -506,146 +633,89 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (e.g. P3:EU -&gt; P5:EU with value: 50%)  </t>
+      <t xml:space="preserve"> or </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">The carbon fraction sheet is only temprorary here and it is being used by thee Flows sheet. In the next version of aiphoria this will be moved. </t>
-  </si>
-  <si>
-    <t>Conversion factor from C to CO2</t>
-  </si>
-  <si>
-    <t>conversion_factor_c_to_co2</t>
-  </si>
-  <si>
-    <t>If using virtual flows, create virtual flow to process if process total inputs and outputs difference is greater than this value</t>
-  </si>
-  <si>
-    <t>virtual_flows_epsilon</t>
-  </si>
-  <si>
-    <t>Use virtual flows. If enabled, creates missing flows for Processes that have imbalance of input and output flows i.e. unreported flows</t>
-  </si>
-  <si>
-    <t>use_virtual_flows</t>
-  </si>
-  <si>
-    <t>Detect the year range automatically from file</t>
-  </si>
-  <si>
-    <t>detect_year_range</t>
-  </si>
-  <si>
-    <t>Ending year of the model, included in in time range</t>
-  </si>
-  <si>
-    <t>end_year</t>
-  </si>
-  <si>
-    <t>Starting year of the model</t>
-  </si>
-  <si>
-    <t>start_year</t>
-  </si>
-  <si>
-    <t>Number of rows to skip when reading data for Processes (e.g. 2). NOTE: Header row must be the first row to read!</t>
-  </si>
-  <si>
-    <t>skip_num_rows_flows</t>
-  </si>
-  <si>
-    <t>Start column name and end column name separated by colon (e.g. B:R) that contain data for Flows</t>
-  </si>
-  <si>
-    <t>B:U</t>
-  </si>
-  <si>
-    <t>column_range_flows</t>
-  </si>
-  <si>
-    <t>Sheet name that contains data for Flows, (e.g. Flows)</t>
-  </si>
-  <si>
-    <t>sheet_name_flows</t>
-  </si>
-  <si>
-    <t>skip_num_rows_processes</t>
-  </si>
-  <si>
-    <t>Start column name and end column name separated by colon (e.g. B:R) that contain data for Processes</t>
-  </si>
-  <si>
-    <t>B:R</t>
-  </si>
-  <si>
-    <t>column_range_processes</t>
-  </si>
-  <si>
-    <t>Sheet name that contains data for Processes, e.g. (Processes)</t>
-  </si>
-  <si>
-    <t>sheet_name_processes</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Parameter name</t>
-  </si>
-  <si>
-    <t>Example: first parameter sheet_name_processes goes to cell B6 and value Processes goes to cell C6.</t>
-  </si>
-  <si>
-    <t>NOTE: The parameters are read columns B and C and from row 7 downward, including that row.</t>
-  </si>
-  <si>
-    <t>These are the settings for the scenario file</t>
-  </si>
-  <si>
-    <t>Boolean values</t>
-  </si>
-  <si>
-    <t>Distribution type</t>
-  </si>
-  <si>
-    <t>fill_missing_absolute_flows</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>Fill in missing timestep with the last timestep provided by the user. Default value is True</t>
-  </si>
-  <si>
-    <t>fill_missing_relative_flows</t>
-  </si>
-  <si>
-    <t>fill_method</t>
-  </si>
-  <si>
-    <t>Previous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String </t>
-  </si>
-  <si>
-    <t>Interpolate</t>
-  </si>
-  <si>
-    <t>Next</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Previous </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zeros </t>
-  </si>
-  <si>
-    <t>Simple</t>
-  </si>
-  <si>
-    <t>Type of fill method</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fill_missing_relative_flows</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is enabled</t>
+    </r>
+  </si>
+  <si>
+    <t>sheet_name_scenarios</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>Sheet name that contains scenarios (flow variations)</t>
+  </si>
+  <si>
+    <t>create_network_graphs</t>
+  </si>
+  <si>
+    <t>Create network graphs to visualize process connections for each scenario</t>
+  </si>
+  <si>
+    <t>create_sankey_charts</t>
+  </si>
+  <si>
+    <t>Create Sankey charts for each scenario</t>
+  </si>
+  <si>
+    <t>Scenario name</t>
+  </si>
+  <si>
+    <t>Source process ID</t>
+  </si>
+  <si>
+    <t>Target process ID</t>
+  </si>
+  <si>
+    <t>Change in value (delta)</t>
+  </si>
+  <si>
+    <t>Target value (potentially)</t>
+  </si>
+  <si>
+    <t>Change type (Value or % = proportional)</t>
+  </si>
+  <si>
+    <t>Start year (included)</t>
+  </si>
+  <si>
+    <t>End year (included)</t>
+  </si>
+  <si>
+    <t>Function type</t>
+  </si>
+  <si>
+    <t>Target process ID (where the opposite change is applied)</t>
+  </si>
+  <si>
+    <t>This sheet contains helper parameters to make changing settings easier inside Excel and to reduce possibilities of typos.</t>
+  </si>
+  <si>
+    <t>All of these settings are strings that can be used as it is in Settings-sheet and in Scenarios-sheet</t>
+  </si>
+  <si>
+    <t>Change type</t>
   </si>
 </sst>
 </file>
@@ -706,14 +776,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="5" tint="0.79998168889431442"/>
       <name val="Calibri"/>
@@ -728,8 +790,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -751,6 +819,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -809,7 +883,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -881,15 +955,18 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -900,15 +977,58 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -950,61 +1070,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>779319</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>64064</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>314785</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>16634</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Graphic 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{060A53AB-2C39-4786-AA4D-FFB36F5549BB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5004955" y="4618746"/>
-          <a:ext cx="9594155" cy="2723479"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1310,7 +1375,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="P3" dT="2024-07-05T06:41:30.02" personId="{10F4E90A-0171-4D8D-A06D-5391EEA853D3}" id="{00ACE76D-287A-45EC-B71C-BD8339701482}">
+  <threadedComment ref="P3" dT="2024-07-05T06:41:30.02" personId="{10F4E90A-0171-4D8D-A06D-5391EEA853D3}" id="{2190F4CE-A9C1-4BF1-8057-C68B26705A49}">
     <text>Conversion to ODMT not carbon!</text>
   </threadedComment>
 </ThreadedComments>
@@ -1321,177 +1386,183 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="18" customWidth="1"/>
     <col min="3" max="3" width="29" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="16"/>
+    <col min="4" max="4" width="69.5703125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="39"/>
-    </row>
-    <row r="2" spans="1:5" ht="156" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="40"/>
+    </row>
+    <row r="2" spans="1:5" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="40"/>
+      <c r="C2" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="41"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="203.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="40"/>
-    </row>
-    <row r="4" spans="1:5" s="17" customFormat="1" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="41"/>
+    </row>
+    <row r="4" spans="1:5" s="17" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="41"/>
-    </row>
-    <row r="5" spans="1:5" s="17" customFormat="1" ht="96.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="42"/>
+    </row>
+    <row r="5" spans="1:5" s="17" customFormat="1" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="41"/>
-    </row>
-    <row r="6" spans="1:5" ht="145" customHeight="1" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="42"/>
+    </row>
+    <row r="6" spans="1:5" ht="144.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="38"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="39"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="42"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="38"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="39"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="38"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="42"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C9" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="38"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="42"/>
-    </row>
-    <row r="11" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
-        <v>52</v>
+        <v>71</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="38"/>
+    </row>
+    <row r="11" spans="1:5" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="D11" s="38"/>
     </row>
-    <row r="12" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D12" s="38"/>
     </row>
-    <row r="13" spans="1:5" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D13" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
@@ -1499,12 +1570,6 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1513,238 +1578,313 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B48F50B1-BB9C-4949-B068-97B97AFD08C4}">
-  <dimension ref="B2:E21"/>
+  <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.81640625" customWidth="1"/>
-    <col min="3" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="103.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="103.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="37" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="36" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
       <c r="E4" s="36"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="35" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C7" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="34" t="s">
+        <v>142</v>
+      </c>
       <c r="E7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="D8" s="34"/>
+        <v>125</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>142</v>
+      </c>
       <c r="E8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C9" s="32">
         <v>2</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="32" t="s">
+        <v>149</v>
+      </c>
       <c r="E9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="34" t="s">
+        <v>150</v>
+      </c>
       <c r="E10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="34"/>
+        <v>119</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>150</v>
+      </c>
       <c r="E11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C12" s="32">
         <v>2</v>
       </c>
-      <c r="D12" s="32"/>
+      <c r="D12" s="32" t="s">
+        <v>149</v>
+      </c>
       <c r="E12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C13" s="32">
         <v>2021</v>
       </c>
-      <c r="D13" s="32"/>
+      <c r="D13" s="32" t="s">
+        <v>149</v>
+      </c>
       <c r="E13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C14" s="32">
         <v>2030</v>
       </c>
-      <c r="D14" s="32"/>
+      <c r="D14" s="32" t="s">
+        <v>149</v>
+      </c>
       <c r="E14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C15" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" t="s">
+        <v>137</v>
+      </c>
       <c r="E15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C16" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="32"/>
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>137</v>
+      </c>
       <c r="E16" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C17" s="31">
         <v>0.1</v>
       </c>
+      <c r="D17" s="32" t="s">
+        <v>151</v>
+      </c>
       <c r="E17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C18" s="30">
         <v>3.67</v>
       </c>
-      <c r="D18" s="30"/>
+      <c r="D18" s="30" t="s">
+        <v>151</v>
+      </c>
       <c r="E18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C19" s="33" t="b">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C20" s="33" t="b">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E20" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" t="s">
         <v>150</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>156</v>
+      </c>
+      <c r="C23" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C15:C16">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="notEqual">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19:C20">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -1752,7 +1892,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:C20">
+  <conditionalFormatting sqref="C23:C24">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -1761,23 +1901,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C19:C20" xr:uid="{5D3B6C52-629A-48C0-B345-97745DEAC80B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C16 C19:C20 C23:C24" xr:uid="{982A8737-D833-4D62-96B8-CE8CEAFA84B7}">
       <formula1>Boolean</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{624030A8-D670-4ECF-A910-6FB291FB46D7}">
-          <x14:formula1>
-            <xm:f>Sheet1!$E$2:$E$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>C21</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1785,30 +1913,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C0D592-75C1-4AD1-84F0-2AAE25CA0097}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="29.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" customWidth="1"/>
-    <col min="9" max="9" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="17.453125" customWidth="1"/>
-    <col min="16" max="16" width="11.81640625" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" customWidth="1"/>
-    <col min="18" max="18" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>9</v>
@@ -1830,7 +1958,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>11</v>
@@ -1860,7 +1988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1886,31 +2014,31 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" s="27" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" s="26" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="J3" s="26" t="s">
         <v>16</v>
@@ -1937,18 +2065,18 @@
         <v>27</v>
       </c>
       <c r="R3" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT(B4,":",C4)</f>
@@ -1961,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1974,18 +2102,18 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="R4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5:D6" si="0">_xlfn.CONCAT(B5,":",C5)</f>
@@ -1998,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -2011,31 +2139,31 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="R5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>Residues:FI</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -2047,18 +2175,18 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="R6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ref="D7" si="1">_xlfn.CONCAT(B7,":",C7)</f>
@@ -2071,7 +2199,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2083,11 +2211,11 @@
         <v>0.53200000000000003</v>
       </c>
       <c r="R7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">
@@ -2101,7 +2229,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution type" prompt="Distribution type for stock outflows (=decay). _x000a_-Fixed only uses lifetimes so no parameter is used._x000a_-Simple only uses lifetimes so no parameter is used._x000a_-Normal, LogNormal, FoldedNormal use standard deviation. _x000a_-Weibull uses shape and scale. " xr:uid="{1B854FDE-0BAE-42E5-8C60-482CEE80872A}">
           <x14:formula1>
-            <xm:f>Sheet1!$C$2:$C$7</xm:f>
+            <xm:f>'Data validation parameters'!$C$2:$C$7</xm:f>
           </x14:formula1>
           <xm:sqref>H4:H1048576</xm:sqref>
         </x14:dataValidation>
@@ -2115,32 +2243,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B692AEE8-68EE-4B81-A49D-50BF066DFFE7}">
   <dimension ref="A1:U91"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="26.54296875" customWidth="1"/>
-    <col min="10" max="10" width="17.81640625" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" customWidth="1"/>
-    <col min="13" max="13" width="40.81640625" customWidth="1"/>
-    <col min="14" max="14" width="21.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="40.85546875" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="94.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2205,7 +2336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2219,7 +2350,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -2228,98 +2359,98 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="20" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C3" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>99</v>
-      </c>
       <c r="I3" s="20" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="M3" s="20" t="s">
         <v>25</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="R3" s="22" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="S3" s="23" t="s">
         <v>21</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="U3" s="23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C4" t="str">
         <f>+_xlfn.XLOOKUP(H4,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Source</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F4" t="str">
         <f>+_xlfn.XLOOKUP(I4,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H4" s="4" t="str">
         <f t="shared" ref="H4:H6" si="0">_xlfn.CONCAT(B4,":",D4)</f>
@@ -2333,45 +2464,45 @@
         <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="L4">
         <v>2021</v>
       </c>
       <c r="N4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="P4">
         <f>0.4238*'Carbon fraction (will be moved)'!$C$2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C5" t="str">
         <f>+_xlfn.XLOOKUP(H5,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F5" t="str">
         <f>+_xlfn.XLOOKUP(I5,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>Second</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2385,45 +2516,45 @@
         <v>50</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="L5">
         <v>2021</v>
       </c>
       <c r="N5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="P5">
         <f>0.4238*'Carbon fraction (will be moved)'!C2</f>
         <v>0.20342399999999999</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C6" t="str">
         <f>+_xlfn.XLOOKUP(H6,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>First</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F6" t="str">
         <f>+_xlfn.XLOOKUP(I6,Processes!$D$4:$D$47,Processes!$E$4:$E$47)</f>
         <v>by_prod</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2437,473 +2568,471 @@
         <v>19.5</v>
       </c>
       <c r="K6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="L6">
         <v>2021</v>
       </c>
       <c r="N6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="P6">
         <f>0.395*'Carbon fraction (will be moved)'!C2</f>
         <v>0.18959999999999999</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="N7"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="N8"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="N9"/>
     </row>
-    <row r="10" spans="1:21" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="N10"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="N11"/>
       <c r="Q11" s="24"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="N12"/>
       <c r="Q12" s="24"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="N13"/>
       <c r="Q13" s="24"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="N14"/>
       <c r="Q14" s="24"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="N15"/>
       <c r="Q15" s="24"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="N16"/>
       <c r="Q16" s="24"/>
     </row>
-    <row r="17" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="N17"/>
       <c r="Q17" s="24"/>
     </row>
-    <row r="18" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="N18"/>
       <c r="Q18" s="24"/>
     </row>
-    <row r="19" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="N21"/>
       <c r="Q21" s="24"/>
     </row>
-    <row r="22" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="N22"/>
       <c r="Q22" s="24"/>
     </row>
-    <row r="23" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="N23"/>
       <c r="Q23" s="24"/>
     </row>
-    <row r="24" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="8:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="O36"/>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="O37"/>
     </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="O38"/>
     </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="N39"/>
       <c r="O39"/>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="N40"/>
       <c r="O40"/>
     </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="N41"/>
       <c r="O41"/>
     </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="N42"/>
       <c r="O42"/>
     </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="N43"/>
       <c r="O43"/>
     </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="N44"/>
       <c r="O44"/>
     </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C45" s="9" t="s">
-        <v>87</v>
-      </c>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C45" s="9"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="N45"/>
       <c r="O45"/>
     </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="N46"/>
       <c r="O46"/>
     </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="N47"/>
       <c r="O47"/>
     </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="N48"/>
       <c r="O48"/>
     </row>
-    <row r="49" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="N49"/>
       <c r="O49"/>
     </row>
-    <row r="50" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="N50"/>
       <c r="O50"/>
     </row>
-    <row r="51" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="N51"/>
       <c r="O51"/>
     </row>
-    <row r="52" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="N52"/>
       <c r="O52"/>
     </row>
-    <row r="53" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="N53"/>
       <c r="O53"/>
     </row>
-    <row r="54" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="N54"/>
       <c r="O54"/>
     </row>
-    <row r="55" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="N55"/>
       <c r="O55"/>
     </row>
-    <row r="56" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="N56"/>
       <c r="O56"/>
     </row>
-    <row r="57" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="N57"/>
       <c r="O57"/>
     </row>
-    <row r="58" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="N58"/>
       <c r="O58"/>
     </row>
-    <row r="59" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="N59"/>
       <c r="O59"/>
     </row>
-    <row r="60" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="N60"/>
       <c r="O60"/>
     </row>
-    <row r="61" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="N61"/>
       <c r="O61"/>
     </row>
-    <row r="62" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="N62"/>
       <c r="O62"/>
     </row>
-    <row r="63" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="N63"/>
       <c r="O63"/>
     </row>
-    <row r="64" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="N64"/>
       <c r="O64"/>
     </row>
-    <row r="65" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="N65"/>
       <c r="O65"/>
     </row>
-    <row r="66" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
       <c r="N66"/>
       <c r="O66"/>
     </row>
-    <row r="67" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="N67"/>
       <c r="O67"/>
     </row>
-    <row r="68" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
       <c r="N68"/>
       <c r="O68"/>
     </row>
-    <row r="69" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
       <c r="N69"/>
       <c r="O69"/>
     </row>
-    <row r="70" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="N70"/>
       <c r="O70"/>
     </row>
-    <row r="71" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="N71"/>
       <c r="O71"/>
     </row>
-    <row r="72" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="N72"/>
       <c r="O72"/>
     </row>
-    <row r="73" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="N73"/>
       <c r="O73"/>
     </row>
-    <row r="74" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="N74"/>
       <c r="O74"/>
     </row>
-    <row r="75" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="N75"/>
       <c r="O75"/>
     </row>
-    <row r="76" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="N76"/>
       <c r="O76"/>
     </row>
-    <row r="77" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="N77"/>
       <c r="O77"/>
     </row>
-    <row r="78" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
       <c r="N78"/>
       <c r="O78"/>
     </row>
-    <row r="79" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="N79"/>
       <c r="O79"/>
     </row>
-    <row r="80" spans="8:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
       <c r="N80"/>
       <c r="O80"/>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
       <c r="N81"/>
       <c r="O81"/>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
       <c r="N82"/>
       <c r="O82"/>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
       <c r="N83"/>
       <c r="O83"/>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
       <c r="N84"/>
       <c r="O84"/>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
       <c r="N85"/>
       <c r="O85"/>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N86"/>
       <c r="O86"/>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -2914,25 +3043,25 @@
       <c r="N87"/>
       <c r="O87"/>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="N88"/>
       <c r="O88"/>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="N89"/>
       <c r="O89"/>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="N90"/>
       <c r="O90"/>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="N91"/>
@@ -2942,44 +3071,68 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1" xr:uid="{44BDC3E8-14C2-47A6-9A94-576E28D9D557}"/>
-    <hyperlink ref="C45" r:id="rId2" location="json=acMq06Ek074LvgJQcBgt-,_z-k-OWtxYKdxCtl_tJVQg " xr:uid="{96378F21-3514-4467-8F52-95C692A9B7F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C620F7-4B8A-4ECD-9835-AFC6C4EF2431}">
-  <dimension ref="B1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A53F7F1-E28C-4890-8454-D65CFA5D529E}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2">
-        <v>0.48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="43" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2988,77 +3141,132 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1385D0A5-68C9-46A8-897F-5695B3E81330}">
-  <dimension ref="C1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C620F7-4B8A-4ECD-9835-AFC6C4EF2431}">
+  <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" customWidth="1"/>
-    <col min="11" max="11" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C1" s="35" t="s">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2">
+        <v>0.48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1385D0A5-68C9-46A8-897F-5695B3E81330}">
+  <dimension ref="B2:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" t="b">
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="b">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>155</v>
+      <c r="D7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3068,12 +3276,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
+    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3340,21 +3551,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="145cc194-9bea-4db6-b116-a042a4529fcd" xsi:nil="true"/>
-    <Comment xmlns="7536dd80-7d39-48e8-9ae3-b4166f580a2d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3379,18 +3596,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{557FAA9C-B184-448F-B58D-00E4D46BDD72}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB3C6F0-DB35-46F0-8FEB-B5E57B48A727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="145cc194-9bea-4db6-b116-a042a4529fcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7536dd80-7d39-48e8-9ae3-b4166f580a2d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>